<commit_message>
添加了 CopyImage, CopyRect, CountClipboardFormats, CreateAcceleratorTable, CreateCaret, CreateCursor, CreateDesktop, CreateDesktopEx 函数
</commit_message>
<xml_diff>
--- a/work_progress/user32.xlsx
+++ b/work_progress/user32.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slime\source\repos\PlatformInvoke\work_progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8019F22F-C32D-476D-BDC8-27BE2552F650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81FFE98-DB64-4101-9EA0-E7913FEE7E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="32220" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="3920" windowWidth="24000" windowHeight="14170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6868" uniqueCount="4511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6879" uniqueCount="4511">
   <si>
     <t>EnumDisplaySettingsExA</t>
   </si>
@@ -13958,10 +13958,10 @@
   <dimension ref="A1:I2249"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D99" sqref="D99"/>
+      <selection pane="bottomRight" activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14000,7 +14000,7 @@
       </c>
       <c r="G1" s="2" t="str">
         <f>"收编: "&amp;TEXT(COUNTIF(E1:E114514, "已完成") + COUNTIF(E1:E114514, "不完善"), "0000")</f>
-        <v>收编: 0073</v>
+        <v>收编: 0083</v>
       </c>
       <c r="H1" s="2" t="str">
         <f>"咕咕咕: "&amp;TEXT(COUNTIF(E1:E114514, "未完成"), "0000")</f>
@@ -14008,7 +14008,7 @@
       </c>
       <c r="I1" s="2" t="str">
         <f>"找不到定义数量: "&amp;TEXT(COUNTIF(E1:E114514, "找不到定义"), "0000")</f>
-        <v>找不到定义数量: 0010</v>
+        <v>找不到定义数量: 0011</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -15662,7 +15662,9 @@
       <c r="D98" s="1" t="s">
         <v>949</v>
       </c>
-      <c r="E98" s="1"/>
+      <c r="E98" s="1" t="s">
+        <v>4488</v>
+      </c>
     </row>
     <row r="99" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
@@ -15677,7 +15679,9 @@
       <c r="D99" s="1" t="s">
         <v>951</v>
       </c>
-      <c r="E99" s="1"/>
+      <c r="E99" s="1" t="s">
+        <v>4488</v>
+      </c>
     </row>
     <row r="100" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
@@ -15692,7 +15696,9 @@
       <c r="D100" s="1" t="s">
         <v>953</v>
       </c>
-      <c r="E100" s="1"/>
+      <c r="E100" s="1" t="s">
+        <v>4488</v>
+      </c>
     </row>
     <row r="101" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
@@ -15707,7 +15713,9 @@
       <c r="D101" s="1" t="s">
         <v>955</v>
       </c>
-      <c r="E101" s="1"/>
+      <c r="E101" s="1" t="s">
+        <v>4488</v>
+      </c>
     </row>
     <row r="102" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
@@ -15722,7 +15730,9 @@
       <c r="D102" s="1" t="s">
         <v>957</v>
       </c>
-      <c r="E102" s="1"/>
+      <c r="E102" s="1" t="s">
+        <v>4488</v>
+      </c>
     </row>
     <row r="103" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
@@ -15737,7 +15747,9 @@
       <c r="D103" s="1" t="s">
         <v>959</v>
       </c>
-      <c r="E103" s="1"/>
+      <c r="E103" s="1" t="s">
+        <v>4488</v>
+      </c>
     </row>
     <row r="104" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
@@ -15752,7 +15764,9 @@
       <c r="D104" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="E104" s="1"/>
+      <c r="E104" s="1" t="s">
+        <v>4488</v>
+      </c>
     </row>
     <row r="105" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
@@ -15767,7 +15781,9 @@
       <c r="D105" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="E105" s="1"/>
+      <c r="E105" s="1" t="s">
+        <v>4488</v>
+      </c>
     </row>
     <row r="106" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
@@ -15782,7 +15798,9 @@
       <c r="D106" s="1" t="s">
         <v>965</v>
       </c>
-      <c r="E106" s="1"/>
+      <c r="E106" s="1" t="s">
+        <v>4487</v>
+      </c>
     </row>
     <row r="107" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
@@ -15797,7 +15815,9 @@
       <c r="D107" s="1" t="s">
         <v>967</v>
       </c>
-      <c r="E107" s="1"/>
+      <c r="E107" s="1" t="s">
+        <v>4488</v>
+      </c>
     </row>
     <row r="108" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
@@ -15842,7 +15862,9 @@
       <c r="D110" s="1" t="s">
         <v>973</v>
       </c>
-      <c r="E110" s="1"/>
+      <c r="E110" s="1" t="s">
+        <v>4488</v>
+      </c>
     </row>
     <row r="111" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">

</xml_diff>